<commit_message>
Programando, para que podamos seleccionar los productos que cumplan con 2 palabras filtro
</commit_message>
<xml_diff>
--- a/BDFisicoQuimicos.xlsx
+++ b/BDFisicoQuimicos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57314\Documents\LEONARDO\CAR\CAR 2022\CONTRATO 2 - 2473\INFORMES VTIC\2. REDES FISICO-QUIMICOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57314\Documents\LEONARDO\CAR\CODIGOS\WebScraping MinCiencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555172D0-A088-4CE2-BE93-9E75EC429BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6BF96D-009B-4CB5-B705-DEDBE0F7A88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FE6734A9-CABE-4AA1-9342-F7E91B507297}"/>
   </bookViews>
@@ -647,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C627B1C-A6CE-4D8F-AF88-8179578616AE}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,207 +766,207 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>67</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>